<commit_message>
Added json, cleaned and merged dataframes. New CSV files added to resources
</commit_message>
<xml_diff>
--- a/Resources/Legal_online_inperson.xlsx
+++ b/Resources/Legal_online_inperson.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8af7e8536f9e44ec/Desktop/Project 3 Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmbla\OneDrive\Desktop\P3\Project-3-Sports-Betting-Analysis\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E4DD35C-12B5-4886-90ED-838FAC795324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57030E0E-6D65-4154-AE5A-0D70439A5941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46560" yWindow="4695" windowWidth="22980" windowHeight="10710" xr2:uid="{D3278CFC-590B-46B3-91F3-3459CEDEF5E9}"/>
+    <workbookView xWindow="-14505" yWindow="-1635" windowWidth="14610" windowHeight="17385" xr2:uid="{D3278CFC-590B-46B3-91F3-3459CEDEF5E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="65">
   <si>
     <t>State</t>
   </si>
@@ -210,6 +210,30 @@
   </si>
   <si>
     <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>ways_to_bet</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Online &amp; In-Person</t>
+  </si>
+  <si>
+    <t>Online Only</t>
+  </si>
+  <si>
+    <t>In-Person Only</t>
+  </si>
+  <si>
+    <t>Pending Both</t>
+  </si>
+  <si>
+    <t>Pending In-Person</t>
+  </si>
+  <si>
+    <t>Pending Online</t>
   </si>
 </sst>
 </file>
@@ -225,12 +249,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,8 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,18 +592,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654C1D0D-50AD-4081-B235-D866F7095F43}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.61328125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,9 +616,12 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -593,9 +630,12 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -604,9 +644,12 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -615,9 +658,12 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -626,9 +672,12 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -637,9 +686,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
@@ -648,9 +700,12 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
@@ -659,460 +714,586 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B43" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>3</v>
       </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B48" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>52</v>
-      </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+      <c r="D49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B50" t="s">
@@ -1121,9 +1302,12 @@
       <c r="C50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+      <c r="D50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B51" t="s">
@@ -1132,9 +1316,12 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+      <c r="D51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B52" t="s">
@@ -1143,9 +1330,16 @@
       <c r="C52" t="s">
         <v>5</v>
       </c>
+      <c r="D52" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C52" xr:uid="{654C1D0D-50AD-4081-B235-D866F7095F43}"/>
+  <autoFilter ref="A1:C52" xr:uid="{654C1D0D-50AD-4081-B235-D866F7095F43}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C52">
+      <sortCondition ref="A1:A52"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>